<commit_message>
Add book assignment and check out file
</commit_message>
<xml_diff>
--- a/ICON360_TCs.xlsx
+++ b/ICON360_TCs.xlsx
@@ -701,7 +701,7 @@
     <xf numFmtId="0" fontId="13" fillId="14" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -952,6 +952,24 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="21" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="20" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="21" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="40">
@@ -11919,7 +11937,7 @@
       </c>
       <c r="G10" s="34" t="inlineStr">
         <is>
-          <t>2023-07-18</t>
+          <t>2023-07-21</t>
         </is>
       </c>
       <c r="H10" s="34" t="inlineStr">
@@ -11977,7 +11995,7 @@
       </c>
       <c r="G11" s="34" t="inlineStr">
         <is>
-          <t>2023-07-17</t>
+          <t>2023-07-21</t>
         </is>
       </c>
       <c r="H11" s="34" t="inlineStr">
@@ -25087,24 +25105,24 @@
           <t>New bondsman information page should be open</t>
         </is>
       </c>
-      <c r="F10" s="32" t="inlineStr">
+      <c r="F10" s="98" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
       <c r="G10" s="34" t="inlineStr">
         <is>
-          <t>2023-28-23</t>
+          <t>2023-07-20</t>
         </is>
       </c>
       <c r="H10" s="34" t="inlineStr">
         <is>
-          <t>Muniba</t>
+          <t>munee</t>
         </is>
       </c>
       <c r="I10" s="34" t="inlineStr">
         <is>
-          <t>Window 10</t>
+          <t>Windows10</t>
         </is>
       </c>
       <c r="J10" s="34" t="inlineStr">
@@ -25112,7 +25130,7 @@
           <t>New bondsman page open</t>
         </is>
       </c>
-      <c r="K10" s="25" t="inlineStr">
+      <c r="K10" s="97" t="inlineStr">
         <is>
           <t>Passed</t>
         </is>
@@ -25143,7 +25161,7 @@
           <t xml:space="preserve">Bondsman should be added </t>
         </is>
       </c>
-      <c r="F11" s="32" t="inlineStr">
+      <c r="F11" s="98" t="inlineStr">
         <is>
           <t>First:john
 Last :wick</t>
@@ -25151,17 +25169,17 @@
       </c>
       <c r="G11" s="34" t="inlineStr">
         <is>
-          <t>2023-28-23</t>
+          <t>2023-07-20</t>
         </is>
       </c>
       <c r="H11" s="34" t="inlineStr">
         <is>
-          <t>Muniba</t>
+          <t>munee</t>
         </is>
       </c>
       <c r="I11" s="34" t="inlineStr">
         <is>
-          <t>Window 10</t>
+          <t>Windows10</t>
         </is>
       </c>
       <c r="J11" s="18" t="inlineStr">
@@ -25169,7 +25187,7 @@
           <t>Bondsome added successfully</t>
         </is>
       </c>
-      <c r="K11" s="25" t="inlineStr">
+      <c r="K11" s="97" t="inlineStr">
         <is>
           <t>Passed</t>
         </is>
@@ -25200,7 +25218,7 @@
           <t xml:space="preserve">It Should be go in main page of bondsman </t>
         </is>
       </c>
-      <c r="F12" s="32" t="inlineStr">
+      <c r="F12" s="98" t="inlineStr">
         <is>
           <t>First:john
 Last :wick</t>
@@ -25208,17 +25226,17 @@
       </c>
       <c r="G12" s="34" t="inlineStr">
         <is>
-          <t>2023-28-23</t>
+          <t>2023-07-20</t>
         </is>
       </c>
       <c r="H12" s="34" t="inlineStr">
         <is>
-          <t>Muniba</t>
+          <t>munee</t>
         </is>
       </c>
       <c r="I12" s="34" t="inlineStr">
         <is>
-          <t>Window 10</t>
+          <t>Windows10</t>
         </is>
       </c>
       <c r="J12" s="34" t="inlineStr">
@@ -25226,7 +25244,7 @@
           <t>User redirected to  back in main page of bondsman</t>
         </is>
       </c>
-      <c r="K12" s="25" t="inlineStr">
+      <c r="K12" s="97" t="inlineStr">
         <is>
           <t>Passed</t>
         </is>
@@ -25306,7 +25324,7 @@
           <t>It not showing the added record</t>
         </is>
       </c>
-      <c r="F14" s="32" t="inlineStr">
+      <c r="F14" s="98" t="inlineStr">
         <is>
           <t>First:john
 Last :wick</t>
@@ -25314,17 +25332,17 @@
       </c>
       <c r="G14" s="34" t="inlineStr">
         <is>
-          <t>2023-28-23</t>
+          <t>2023-07-20</t>
         </is>
       </c>
       <c r="H14" s="34" t="inlineStr">
         <is>
-          <t>Muniba</t>
+          <t>munee</t>
         </is>
       </c>
       <c r="I14" s="34" t="inlineStr">
         <is>
-          <t>Window 10</t>
+          <t>Windows10</t>
         </is>
       </c>
       <c r="J14" s="18" t="inlineStr">
@@ -25332,9 +25350,9 @@
           <t xml:space="preserve">Correct data found </t>
         </is>
       </c>
-      <c r="K14" s="25" t="inlineStr">
-        <is>
-          <t>Failed</t>
+      <c r="K14" s="97" t="inlineStr">
+        <is>
+          <t>Passed</t>
         </is>
       </c>
     </row>
@@ -25361,24 +25379,24 @@
           <t xml:space="preserve">it should show that no record found </t>
         </is>
       </c>
-      <c r="F15" s="18" t="inlineStr">
+      <c r="F15" s="99" t="inlineStr">
         <is>
           <t xml:space="preserve">*12  in bondsmans  search box </t>
         </is>
       </c>
       <c r="G15" s="34" t="inlineStr">
         <is>
-          <t>2023-28-23</t>
+          <t>2023-07-20</t>
         </is>
       </c>
       <c r="H15" s="34" t="inlineStr">
         <is>
-          <t>Muniba</t>
+          <t>munee</t>
         </is>
       </c>
       <c r="I15" s="34" t="inlineStr">
         <is>
-          <t>Window 10</t>
+          <t>Windows10</t>
         </is>
       </c>
       <c r="J15" s="18" t="inlineStr">
@@ -25386,7 +25404,7 @@
           <t>It shows no record found</t>
         </is>
       </c>
-      <c r="K15" s="25" t="inlineStr">
+      <c r="K15" s="97" t="inlineStr">
         <is>
           <t>Passed</t>
         </is>
@@ -25421,7 +25439,7 @@
           <t xml:space="preserve">information should be updated but no text message received </t>
         </is>
       </c>
-      <c r="F16" s="36" t="inlineStr">
+      <c r="F16" s="99" t="inlineStr">
         <is>
           <t>First:john
 Last :wick</t>
@@ -25429,17 +25447,17 @@
       </c>
       <c r="G16" s="34" t="inlineStr">
         <is>
-          <t>2023-28-23</t>
+          <t>2023-07-20</t>
         </is>
       </c>
       <c r="H16" s="34" t="inlineStr">
         <is>
-          <t>Muniba</t>
+          <t>munee</t>
         </is>
       </c>
       <c r="I16" s="34" t="inlineStr">
         <is>
-          <t>Window 10</t>
+          <t>Windows10</t>
         </is>
       </c>
       <c r="J16" s="18" t="inlineStr">
@@ -25447,7 +25465,7 @@
           <t xml:space="preserve">Information updated </t>
         </is>
       </c>
-      <c r="K16" s="25" t="inlineStr">
+      <c r="K16" s="97" t="inlineStr">
         <is>
           <t>Passed</t>
         </is>
@@ -25481,24 +25499,24 @@
           <t>It should not be deleted because it linked mutiple cases but it deleted .need your criteria</t>
         </is>
       </c>
-      <c r="F17" s="18" t="n"/>
+      <c r="F17" s="99" t="n"/>
       <c r="G17" s="34" t="inlineStr">
         <is>
-          <t>2023-28-23</t>
+          <t>2023-07-20</t>
         </is>
       </c>
       <c r="H17" s="34" t="inlineStr">
         <is>
-          <t>Muniba</t>
+          <t>munee</t>
         </is>
       </c>
       <c r="I17" s="34" t="inlineStr">
         <is>
-          <t>Window 10</t>
+          <t>Windows10</t>
         </is>
       </c>
       <c r="J17" s="18" t="n"/>
-      <c r="K17" s="25" t="inlineStr">
+      <c r="K17" s="97" t="inlineStr">
         <is>
           <t>Passed</t>
         </is>
@@ -30622,30 +30640,30 @@
           <t xml:space="preserve">it should not open new page only exited box slightly move to left (need the accptenace criteria) </t>
         </is>
       </c>
-      <c r="F10" s="32" t="inlineStr">
+      <c r="F10" s="98" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
       <c r="G10" s="34" t="inlineStr">
         <is>
-          <t>2023-28-23</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="H10" s="34" t="inlineStr">
         <is>
-          <t>Muniba</t>
+          <t>munee</t>
         </is>
       </c>
       <c r="I10" s="34" t="inlineStr">
         <is>
-          <t>Window 10</t>
+          <t>Windows10</t>
         </is>
       </c>
       <c r="J10" s="34" t="n"/>
-      <c r="K10" s="39" t="inlineStr">
-        <is>
-          <t>sed</t>
+      <c r="K10" s="101" t="inlineStr">
+        <is>
+          <t>Passed</t>
         </is>
       </c>
     </row>
@@ -30731,20 +30749,20 @@
           <t>it Should be reset Book page Assignment</t>
         </is>
       </c>
-      <c r="F12" s="32" t="n"/>
+      <c r="F12" s="98" t="n"/>
       <c r="G12" s="34" t="inlineStr">
         <is>
-          <t>2023-28-23</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="H12" s="34" t="inlineStr">
         <is>
-          <t>Muniba</t>
+          <t>munee</t>
         </is>
       </c>
       <c r="I12" s="34" t="inlineStr">
         <is>
-          <t>Window 10</t>
+          <t>Windows10</t>
         </is>
       </c>
       <c r="J12" s="34" t="inlineStr">
@@ -30752,9 +30770,9 @@
           <t>all the input fields are rest</t>
         </is>
       </c>
-      <c r="K12" s="43" t="inlineStr">
-        <is>
-          <t>Passed</t>
+      <c r="K12" s="104" t="inlineStr">
+        <is>
+          <t>Failed</t>
         </is>
       </c>
     </row>
@@ -30834,24 +30852,24 @@
           <t xml:space="preserve">information should be updated but no text message received </t>
         </is>
       </c>
-      <c r="F14" s="36" t="inlineStr">
+      <c r="F14" s="99" t="inlineStr">
         <is>
           <t>page:100</t>
         </is>
       </c>
       <c r="G14" s="34" t="inlineStr">
         <is>
-          <t>2023-28-23</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="H14" s="34" t="inlineStr">
         <is>
-          <t>Muniba</t>
+          <t>munee</t>
         </is>
       </c>
       <c r="I14" s="34" t="inlineStr">
         <is>
-          <t>Window 10</t>
+          <t>Windows10</t>
         </is>
       </c>
       <c r="J14" s="18" t="inlineStr">
@@ -30859,7 +30877,7 @@
           <t xml:space="preserve">information updated </t>
         </is>
       </c>
-      <c r="K14" s="43" t="inlineStr">
+      <c r="K14" s="103" t="inlineStr">
         <is>
           <t>Passed</t>
         </is>
@@ -30892,24 +30910,24 @@
           <t>it should be deleted</t>
         </is>
       </c>
-      <c r="F15" s="18" t="n"/>
+      <c r="F15" s="99" t="n"/>
       <c r="G15" s="34" t="inlineStr">
         <is>
-          <t>2023-28-23</t>
+          <t>2023-07-24</t>
         </is>
       </c>
       <c r="H15" s="34" t="inlineStr">
         <is>
-          <t>Muniba</t>
+          <t>munee</t>
         </is>
       </c>
       <c r="I15" s="34" t="inlineStr">
         <is>
-          <t>Window 10</t>
+          <t>Windows10</t>
         </is>
       </c>
       <c r="J15" s="18" t="n"/>
-      <c r="K15" s="43" t="inlineStr">
+      <c r="K15" s="103" t="inlineStr">
         <is>
           <t>Passed</t>
         </is>
@@ -32315,24 +32333,24 @@
           <t xml:space="preserve">It should all case file check out cases </t>
         </is>
       </c>
-      <c r="F10" s="32" t="inlineStr">
+      <c r="F10" s="98" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
       <c r="G10" s="34" t="inlineStr">
         <is>
-          <t>2023-28-23</t>
+          <t>2023-07-25</t>
         </is>
       </c>
       <c r="H10" s="34" t="inlineStr">
         <is>
-          <t>Muniba</t>
+          <t>munee</t>
         </is>
       </c>
       <c r="I10" s="34" t="inlineStr">
         <is>
-          <t>Window 10</t>
+          <t>Windows10</t>
         </is>
       </c>
       <c r="J10" s="34" t="inlineStr">
@@ -32340,7 +32358,7 @@
           <t>All check out cases shown in main page</t>
         </is>
       </c>
-      <c r="K10" s="25" t="inlineStr">
+      <c r="K10" s="97" t="inlineStr">
         <is>
           <t>Passed</t>
         </is>
@@ -32370,24 +32388,24 @@
           <t>It should display the data against relevnt case no</t>
         </is>
       </c>
-      <c r="F11" s="32" t="inlineStr">
+      <c r="F11" s="98" t="inlineStr">
         <is>
           <t>Contains:16CV00510 any correct case that is checked out</t>
         </is>
       </c>
       <c r="G11" s="34" t="inlineStr">
         <is>
-          <t>2023-28-23</t>
+          <t>2023-07-25</t>
         </is>
       </c>
       <c r="H11" s="34" t="inlineStr">
         <is>
-          <t>Muniba</t>
+          <t>munee</t>
         </is>
       </c>
       <c r="I11" s="34" t="inlineStr">
         <is>
-          <t>Window 10</t>
+          <t>Windows10</t>
         </is>
       </c>
       <c r="J11" s="33" t="inlineStr">
@@ -32395,7 +32413,7 @@
           <t>Correct information retrived</t>
         </is>
       </c>
-      <c r="K11" s="25" t="inlineStr">
+      <c r="K11" s="97" t="inlineStr">
         <is>
           <t>Passed</t>
         </is>
@@ -32426,24 +32444,24 @@
 (but there should be not record found instead of empty )</t>
         </is>
       </c>
-      <c r="F12" s="32" t="inlineStr">
+      <c r="F12" s="98" t="inlineStr">
         <is>
           <t>Contains:Any incorrect case that is  not checked out</t>
         </is>
       </c>
       <c r="G12" s="34" t="inlineStr">
         <is>
-          <t>2023-28-23</t>
+          <t>2023-07-25</t>
         </is>
       </c>
       <c r="H12" s="34" t="inlineStr">
         <is>
-          <t>Muniba</t>
+          <t>munee</t>
         </is>
       </c>
       <c r="I12" s="34" t="inlineStr">
         <is>
-          <t>Window 10</t>
+          <t>Windows10</t>
         </is>
       </c>
       <c r="J12" s="33" t="inlineStr">
@@ -32451,7 +32469,7 @@
           <t>No data retrived</t>
         </is>
       </c>
-      <c r="K12" s="25" t="inlineStr">
+      <c r="K12" s="97" t="inlineStr">
         <is>
           <t>Passed</t>
         </is>
@@ -32481,24 +32499,24 @@
           <t>It should display the data against relevnt judge</t>
         </is>
       </c>
-      <c r="F13" s="32" t="inlineStr">
+      <c r="F13" s="98" t="inlineStr">
         <is>
           <t>Contains any correct Judge that is  not checked out</t>
         </is>
       </c>
       <c r="G13" s="34" t="inlineStr">
         <is>
-          <t>2023-28-23</t>
+          <t>2023-07-25</t>
         </is>
       </c>
       <c r="H13" s="34" t="inlineStr">
         <is>
-          <t>Muniba</t>
+          <t>munee</t>
         </is>
       </c>
       <c r="I13" s="34" t="inlineStr">
         <is>
-          <t>Window 10</t>
+          <t>Windows10</t>
         </is>
       </c>
       <c r="J13" s="33" t="inlineStr">
@@ -32506,7 +32524,7 @@
           <t>Correct information retrived</t>
         </is>
       </c>
-      <c r="K13" s="25" t="inlineStr">
+      <c r="K13" s="97" t="inlineStr">
         <is>
           <t>Passed</t>
         </is>
@@ -32537,24 +32555,24 @@
 (but there should be not record found instead of empty )</t>
         </is>
       </c>
-      <c r="F14" s="32" t="inlineStr">
+      <c r="F14" s="98" t="inlineStr">
         <is>
           <t>Contains:any incorrect judge that is  not checked out</t>
         </is>
       </c>
       <c r="G14" s="34" t="inlineStr">
         <is>
-          <t>2023-28-23</t>
+          <t>2023-07-25</t>
         </is>
       </c>
       <c r="H14" s="34" t="inlineStr">
         <is>
-          <t>Muniba</t>
+          <t>munee</t>
         </is>
       </c>
       <c r="I14" s="34" t="inlineStr">
         <is>
-          <t>Window 10</t>
+          <t>Windows10</t>
         </is>
       </c>
       <c r="J14" s="33" t="inlineStr">
@@ -32562,7 +32580,7 @@
           <t>No data retrived</t>
         </is>
       </c>
-      <c r="K14" s="25" t="inlineStr">
+      <c r="K14" s="97" t="inlineStr">
         <is>
           <t>Passed</t>
         </is>
@@ -32592,24 +32610,24 @@
           <t>It should display the data against relevnt Days out</t>
         </is>
       </c>
-      <c r="F15" s="32" t="inlineStr">
+      <c r="F15" s="98" t="inlineStr">
         <is>
           <t>Contains any correct Days out</t>
         </is>
       </c>
       <c r="G15" s="34" t="inlineStr">
         <is>
-          <t>2023-28-23</t>
+          <t>2023-07-25</t>
         </is>
       </c>
       <c r="H15" s="34" t="inlineStr">
         <is>
-          <t>Muniba</t>
+          <t>munee</t>
         </is>
       </c>
       <c r="I15" s="34" t="inlineStr">
         <is>
-          <t>Window 10</t>
+          <t>Windows10</t>
         </is>
       </c>
       <c r="J15" s="33" t="inlineStr">
@@ -32617,7 +32635,7 @@
           <t>Correct information retrived</t>
         </is>
       </c>
-      <c r="K15" s="25" t="inlineStr">
+      <c r="K15" s="97" t="inlineStr">
         <is>
           <t>Passed</t>
         </is>
@@ -32759,24 +32777,24 @@
 (but there should be not record found instead of empty )</t>
         </is>
       </c>
-      <c r="F18" s="32" t="inlineStr">
+      <c r="F18" s="98" t="inlineStr">
         <is>
           <t>Contains:any incorrect User that is  not checked out</t>
         </is>
       </c>
       <c r="G18" s="34" t="inlineStr">
         <is>
-          <t>2023-28-23</t>
+          <t>2023-07-25</t>
         </is>
       </c>
       <c r="H18" s="34" t="inlineStr">
         <is>
-          <t>Muniba</t>
+          <t>munee</t>
         </is>
       </c>
       <c r="I18" s="34" t="inlineStr">
         <is>
-          <t>Window 10</t>
+          <t>Windows10</t>
         </is>
       </c>
       <c r="J18" s="33" t="inlineStr">
@@ -32784,7 +32802,7 @@
           <t>No data retrived</t>
         </is>
       </c>
-      <c r="K18" s="25" t="inlineStr">
+      <c r="K18" s="97" t="inlineStr">
         <is>
           <t>Passed</t>
         </is>
@@ -32816,7 +32834,7 @@
           <t>It should created the badge label</t>
         </is>
       </c>
-      <c r="F19" s="26" t="inlineStr">
+      <c r="F19" s="105" t="inlineStr">
         <is>
           <t>borrowers:Muniba
 borrowers office/organization :self</t>
@@ -32824,17 +32842,17 @@
       </c>
       <c r="G19" s="34" t="inlineStr">
         <is>
-          <t>2023-28-23</t>
+          <t>2023-07-25</t>
         </is>
       </c>
       <c r="H19" s="34" t="inlineStr">
         <is>
-          <t>Muniba</t>
+          <t>munee</t>
         </is>
       </c>
       <c r="I19" s="34" t="inlineStr">
         <is>
-          <t>Window 10</t>
+          <t>Windows10</t>
         </is>
       </c>
       <c r="J19" s="45" t="inlineStr">
@@ -32842,7 +32860,7 @@
           <t>Bagde label created</t>
         </is>
       </c>
-      <c r="K19" s="25" t="inlineStr">
+      <c r="K19" s="97" t="inlineStr">
         <is>
           <t>Passed</t>
         </is>
@@ -32929,24 +32947,24 @@
           <t>Data should be export exceld</t>
         </is>
       </c>
-      <c r="F21" s="46" t="inlineStr">
+      <c r="F21" s="106" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
       </c>
       <c r="G21" s="34" t="inlineStr">
         <is>
-          <t>2023-28-23</t>
+          <t>2023-07-25</t>
         </is>
       </c>
       <c r="H21" s="34" t="inlineStr">
         <is>
-          <t>Muniba</t>
+          <t>munee</t>
         </is>
       </c>
       <c r="I21" s="34" t="inlineStr">
         <is>
-          <t>Window 10</t>
+          <t>Windows10</t>
         </is>
       </c>
       <c r="J21" s="45" t="inlineStr">
@@ -32954,7 +32972,7 @@
           <t xml:space="preserve">Correct data exported </t>
         </is>
       </c>
-      <c r="K21" s="25" t="inlineStr">
+      <c r="K21" s="97" t="inlineStr">
         <is>
           <t>Passed</t>
         </is>

</xml_diff>